<commit_message>
tested and fixed issues with build_fem_data. added a new function plot_fem_data to show fem mesh with boundary condition symbols
</commit_message>
<xml_diff>
--- a/inputs/slope/input_template_lface6.xlsx
+++ b/inputs/slope/input_template_lface6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/cursor_projects/xslope/inputs/slope/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65044D8-BFEE-4B42-BA33-2C7711F96F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D226CC9-9DD3-8A48-9978-FE1641E4B874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23460" yWindow="1840" windowWidth="34160" windowHeight="22520" activeTab="3" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="23460" yWindow="1840" windowWidth="34160" windowHeight="22520" activeTab="7" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -2025,6 +2025,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>220</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2034,6 +2040,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>84</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -5888,7 +5900,7 @@
   <dimension ref="A2:N38"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6417,16 +6429,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="M22:N22"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="M4:N4"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="M22:N22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6436,7 +6448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA88A0E-2BF5-FE49-9603-08BE4D91829B}">
   <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -7708,8 +7720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7976BB56-7732-404C-B58A-55DA7F8052B3}">
   <dimension ref="B2:P29"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7785,9 +7797,15 @@
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="B4" s="3">
+        <v>170</v>
+      </c>
+      <c r="C4" s="3">
+        <v>84</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1000</v>
+      </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -7799,9 +7817,15 @@
       <c r="P4" s="3"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="B5" s="3">
+        <v>220</v>
+      </c>
+      <c r="C5" s="3">
+        <v>84</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1000</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>

</xml_diff>

<commit_message>
debugged solve_fem function. fixed bug in build_polygons when there is only one profile line.
</commit_message>
<xml_diff>
--- a/inputs/slope/input_template_lface6.xlsx
+++ b/inputs/slope/input_template_lface6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/cursor_projects/xslope/inputs/slope/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D226CC9-9DD3-8A48-9978-FE1641E4B874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B64626F-73A0-594E-8920-F345B12DE6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23460" yWindow="1840" windowWidth="34160" windowHeight="22520" activeTab="7" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
@@ -2025,12 +2025,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>220</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2040,12 +2034,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>84</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6429,16 +6417,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="M4:N4"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="M22:N22"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="M4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7721,7 +7709,7 @@
   <dimension ref="B2:P29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7797,15 +7785,9 @@
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B4" s="3">
-        <v>170</v>
-      </c>
-      <c r="C4" s="3">
-        <v>84</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1000</v>
-      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -7817,15 +7799,9 @@
       <c r="P4" s="3"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B5" s="3">
-        <v>220</v>
-      </c>
-      <c r="C5" s="3">
-        <v>84</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1000</v>
-      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>

</xml_diff>